<commit_message>
Update ISE 1 Maths, Noms et email.xlsx
</commit_message>
<xml_diff>
--- a/ISE 1 Maths, Noms et email.xlsx
+++ b/ISE 1 Maths, Noms et email.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DYVANA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/a_hema_cgiar_org/Documents/Desktop/Cours/2025/ENSAE/Projet statistique sous R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7485DF-62E4-47B7-BAEC-A25781B93340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{DA7485DF-62E4-47B7-BAEC-A25781B93340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE67EF88-9397-44D0-9CD1-645DA3E94FF5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7411E553-FC8F-4234-965D-938F8A2CDC11}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7411E553-FC8F-4234-965D-938F8A2CDC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -163,9 +163,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,7 +203,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -309,7 +309,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,7 +451,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,18 +462,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="4" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="4" max="5" width="31.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -490,7 +490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -510,7 +510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -530,7 +530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -547,7 +547,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>

</xml_diff>